<commit_message>
Working on feedback points
</commit_message>
<xml_diff>
--- a/src/assets/samplefiles/FI_USERS.xlsx
+++ b/src/assets/samplefiles/FI_USERS.xlsx
@@ -23,9 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">National ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">Número de cédula</t>
   </si>
   <si>
     <t xml:space="preserve">Correo electrónico</t>
@@ -34,31 +34,13 @@
     <t xml:space="preserve">Código del país</t>
   </si>
   <si>
-    <t xml:space="preserve">Teléfono</t>
+    <t xml:space="preserve">Número de celular</t>
   </si>
   <si>
     <t xml:space="preserve">RUC de la Entidad</t>
   </si>
   <si>
     <t xml:space="preserve">Role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chica.garces@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADMIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mejia.lopez@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AGENT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moyano.allan@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">caiza.pillajo@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -68,7 +50,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -99,12 +81,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -148,7 +124,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -159,10 +135,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -203,20 +175,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1009" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -240,70 +212,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1309895330</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>2390002230001</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
-        <v>1002241147</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>2390002230001</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1712993938</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>1791375874001</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>1716194319</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>1791375874001</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="F1:F3"/>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="chica.garces@yopmail.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="mejia.lopez@yopmail.com"/>
-    <hyperlink ref="B4" r:id="rId3" display="moyano.allan@yopmail.com"/>
-    <hyperlink ref="B5" r:id="rId4" display="caiza.pillajo@yopmail.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -311,7 +221,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>